<commit_message>
Added the resizer module
</commit_message>
<xml_diff>
--- a/diagrams/module-status.xlsx
+++ b/diagrams/module-status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Module Name</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>Permite realizarea unor animatii mai complexe on hover. E folosita la meniul din header si la our clients.</t>
+  </si>
+  <si>
+    <t>app.fancy-slider.resizer</t>
+  </si>
+  <si>
+    <t>In functie de rezolutia maxima si minima definita, acesta calculeaza scalarea sliderul pentru a ocupa tot ecranul.</t>
   </si>
 </sst>
 </file>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +432,7 @@
     <col min="1" max="1" width="32.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="92.28515625" customWidth="1"/>
+    <col min="5" max="5" width="101.28515625" customWidth="1"/>
     <col min="6" max="6" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -449,56 +455,67 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added the controls module
</commit_message>
<xml_diff>
--- a/diagrams/module-status.xlsx
+++ b/diagrams/module-status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Module Name</t>
   </si>
@@ -65,13 +65,22 @@
   </si>
   <si>
     <t>In functie de rezolutia maxima si minima definita, acesta calculeaza scalarea sliderul pentru a ocupa tot ecranul.</t>
+  </si>
+  <si>
+    <t>app.fancy-slider.controls</t>
+  </si>
+  <si>
+    <t>Trebuie integrat!</t>
+  </si>
+  <si>
+    <t>Ii comunica "Creierului" in ce directie vrea userul sa schimbe sliderul.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,8 +95,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,6 +113,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -109,16 +130,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -421,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,67 +479,80 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added the blur module (incomplete)
</commit_message>
<xml_diff>
--- a/diagrams/module-status.xlsx
+++ b/diagrams/module-status.xlsx
@@ -10,11 +10,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Module Name</t>
   </si>
@@ -101,6 +102,12 @@
   </si>
   <si>
     <t>app.fancy-slider.slide</t>
+  </si>
+  <si>
+    <t>app.fancy-slider.blur</t>
+  </si>
+  <si>
+    <t>Nu-I complet!</t>
   </si>
 </sst>
 </file>
@@ -472,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,114 +529,126 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Integrated the fancy slider's controls
</commit_message>
<xml_diff>
--- a/diagrams/module-status.xlsx
+++ b/diagrams/module-status.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Module Name</t>
   </si>
@@ -482,7 +481,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,13 +542,9 @@
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="D5" s="1"/>
       <c r="E5" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Updated the slides module
I've made all the needed changes as I'm preparing to integrate velocity!
</commit_message>
<xml_diff>
--- a/diagrams/module-status.xlsx
+++ b/diagrams/module-status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Module Name</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Nu-I complet!</t>
+  </si>
+  <si>
+    <t>O metoda rapida de a incarca fiecare slide</t>
   </si>
 </sst>
 </file>
@@ -480,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,6 +583,9 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">

</xml_diff>

<commit_message>
The blur module implements velocity
</commit_message>
<xml_diff>
--- a/diagrams/module-status.xlsx
+++ b/diagrams/module-status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Module Name</t>
   </si>
@@ -106,10 +106,10 @@
     <t>app.fancy-slider.blur</t>
   </si>
   <si>
-    <t>Nu-I complet!</t>
-  </si>
-  <si>
     <t>O metoda rapida de a incarca fiecare slide</t>
+  </si>
+  <si>
+    <t>Ii da creierului functia posibilitatea de a blura!</t>
   </si>
 </sst>
 </file>
@@ -483,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,12 +533,11 @@
       <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
+      <c r="D4" s="1"/>
+      <c r="E4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -584,7 +583,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated module-status to showcase the latest changes
</commit_message>
<xml_diff>
--- a/diagrams/module-status.xlsx
+++ b/diagrams/module-status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Module Name</t>
   </si>
@@ -104,6 +104,24 @@
   </si>
   <si>
     <t>Contine toate animatiile fiecarei resurse! El ii ofera creierului o serie de controale!</t>
+  </si>
+  <si>
+    <t>common.gsap-lite</t>
+  </si>
+  <si>
+    <t>Incapsuleaza TweenLite si Easing'urile.</t>
+  </si>
+  <si>
+    <t>common.viewport-size</t>
+  </si>
+  <si>
+    <t>Ne ofera acces la resolutia curenta a viewportului. Totodata ne ofera posibilitatea de a registra callbackuri.</t>
+  </si>
+  <si>
+    <t>common.pixi</t>
+  </si>
+  <si>
+    <t>Incapsuleaza pixi.js.</t>
   </si>
 </sst>
 </file>
@@ -475,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,45 +618,78 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the diagram and module status
</commit_message>
<xml_diff>
--- a/diagrams/module-status.xlsx
+++ b/diagrams/module-status.xlsx
@@ -40,15 +40,9 @@
     <t>common.retina-images</t>
   </si>
   <si>
-    <t>state.preloader</t>
-  </si>
-  <si>
     <t>Best-practicy JS</t>
   </si>
   <si>
-    <t>Acesta e primul lucru pe care un utilizator il vede cand intra pe site.</t>
-  </si>
-  <si>
     <t>Ofera functionalitatea de baza pentru a ne creea liste de descarcare.</t>
   </si>
   <si>
@@ -106,9 +100,6 @@
     <t>common.gsap-lite</t>
   </si>
   <si>
-    <t>Incapsuleaza TweenLite si Easing'urile.</t>
-  </si>
-  <si>
     <t>common.viewport-size</t>
   </si>
   <si>
@@ -122,6 +113,15 @@
   </si>
   <si>
     <t>Compus din 3 componente: un inline script pus in &lt;head&gt;, un modul in .htaccess si o constanta angular IS_RETINA ce ne zice daca device'ul utilizatorului e retina sau nu.</t>
+  </si>
+  <si>
+    <t>Incapsuleaza TweenLite, TimelineLite si Easing'urile (Power1, Power2, Power3, Power4)</t>
+  </si>
+  <si>
+    <t>app.fancy-slider.assets-downloader</t>
+  </si>
+  <si>
+    <t>Foloseste preloader'ul pentru a crea o lista de descarcare. Cand preloaderul termina descarcarea, acesta mai infasoara odata resursele intr-un loader PIXI pentru a ne asigura ca acestea sunt si in cache'ul pixi.</t>
   </si>
 </sst>
 </file>
@@ -493,15 +493,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="27.85546875" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
@@ -520,7 +520,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -528,169 +528,169 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="D6" s="1"/>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>22</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>